<commit_message>
Large commit - add size to ud pos languages, analysing UD POS predictions for Dutch, creating a dataset for calculating feature importance, add two letter language abbreviations to xtreme_langs.xlsx
</commit_message>
<xml_diff>
--- a/code/xtreme_langs_wals_with_data_size.xlsx
+++ b/code/xtreme_langs_wals_with_data_size.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bdolicki\Documents\Git\multilingual-analysis\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3956F09B-AE3C-4104-A5DD-72A0C7F60C94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{219132D1-3C0F-4A64-B106-BF9BE831CDE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16690" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2964,7 +2964,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:GC43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Refactoring and comparing base vs large model for NER. - Refactor analysing predictions to reduce code repetition and created utils.py that is imported in every relevant notebook. - Rename EN results for UDPOS. - Refactor the notebook "Comparing base to large...", added results from PANX and renamed it.
</commit_message>
<xml_diff>
--- a/code/xtreme_langs_wals_with_data_size.xlsx
+++ b/code/xtreme_langs_wals_with_data_size.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bdolicki\Documents\Git\multilingual-analysis\code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bdolicki\Documents\Git\multilingual-analysis\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{219132D1-3C0F-4A64-B106-BF9BE831CDE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E2ABFB-4EBA-48C8-A1A1-C0C429C157DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="18900" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2965,10 +2965,13 @@
   <dimension ref="A1:GC43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="5" width="24.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:185" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">

</xml_diff>